<commit_message>
add sql & kmeans segmentation
</commit_message>
<xml_diff>
--- a/mybook/ch3_pandas/my_cheatsheet.xlsx
+++ b/mybook/ch3_pandas/my_cheatsheet.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/我的雲端硬碟/0. codepool_python/python_ds/mybook/ch3_pandas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB83627-FC92-3E44-804F-4E29A9652F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CAB93D-3BB0-1E44-9AFE-519227415B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="4" xr2:uid="{04BD9F13-8DC2-274D-9BB0-10DA52A0F654}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{04BD9F13-8DC2-274D-9BB0-10DA52A0F654}"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="1" r:id="rId1"/>
-    <sheet name="overview" sheetId="4" r:id="rId2"/>
-    <sheet name="random" sheetId="12" r:id="rId3"/>
-    <sheet name="summarise" sheetId="8" r:id="rId4"/>
-    <sheet name="select_filter_arrange_mutate" sheetId="6" r:id="rId5"/>
-    <sheet name="subset&amp;slice" sheetId="5" r:id="rId6"/>
-    <sheet name="group_by特輯" sheetId="7" r:id="rId7"/>
-    <sheet name="missing_data" sheetId="9" r:id="rId8"/>
-    <sheet name="combine" sheetId="10" r:id="rId9"/>
-    <sheet name="pipe" sheetId="13" r:id="rId10"/>
-    <sheet name="單元測試" sheetId="14" r:id="rId11"/>
+    <sheet name="datetime" sheetId="15" r:id="rId2"/>
+    <sheet name="overview" sheetId="4" r:id="rId3"/>
+    <sheet name="random" sheetId="12" r:id="rId4"/>
+    <sheet name="summarise" sheetId="8" r:id="rId5"/>
+    <sheet name="select_filter_arrange_mutate" sheetId="6" r:id="rId6"/>
+    <sheet name="subset&amp;slice" sheetId="5" r:id="rId7"/>
+    <sheet name="group_by特輯" sheetId="7" r:id="rId8"/>
+    <sheet name="missing_data" sheetId="9" r:id="rId9"/>
+    <sheet name="combine" sheetId="10" r:id="rId10"/>
+    <sheet name="pipe" sheetId="13" r:id="rId11"/>
+    <sheet name="單元測試" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="383">
   <si>
     <t>R</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1737,12 +1738,560 @@
   .apply(lambda x: x.iloc[:5])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Matlab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>summary(df)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sortrows(df, "a")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sortrows(df, "a", "descend")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sortrows(df, ["col1", "col2"])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(1, 2) % 第一列，第二行
+df(1, "行名2")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df([1,2], [1,2])
+df([1,2], ["行名1", "行名2"])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, [1,2])
+df(:, ["行名1", "行名2"])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df{1, 2} % 第一列，第二行
+df{1, "行名2"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, 2:7)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(2:7, :)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df([1,3], :)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, "col1")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, ["col1", "col2"])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, [1:2])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, [1, 3, 5])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, end-2:end)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df(:, ["col1", "col2"]) = []</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把 C 欄位排到 A 欄前面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df = movevars(df, "C", "Before", "A")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把 C 欄位排到 A 欄後面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df = movevars(df, "C", "After", "A")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df.new = 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df.c = df.a + df.b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df.Properties.VariableNames</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R (lubridate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parse date time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017-01-31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07-04-2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20210223 10:00:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">取 date: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>2018-01-31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 14:00:00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get components</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取 week: 2018-01-31 14:00:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取 quarter: 2018-01-31 14:00:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">取 year: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>2018</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>-01-31 14:00:00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>取 month: 2018-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>-31 14:00:00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>取 day: 2018-01-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> 14:00:00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">取 hour: 2018-01-31 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>:00:00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>取 minute: 2018-01-31 14:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>:00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>取 second: 2018-01-31 14:00:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x = ymd_hms("2018-01-31 14:00:00")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>month(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hour(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minute(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>second(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>week(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quarter(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d = ymd("20170131", tz = "Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d = ymd("2017-01-31", tz = "Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d = mdy("July 4th, 2000", tz = "Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d = mdy("07-04-2021", tz = "Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d = ymd_hms("20210223 10:00:00", tz = "Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime(a, "InputFormat", "yyyy-MM-dd HH:mm:ss", "TimeZone","Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018-01-31 14:00:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime(a, "InputFormat", "yyyyMMdd HH:mm:ss", "TimeZone","Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime(a, "InputFormat", "MM-dd-yyyy", "TimeZone","Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a = "April 14, 2000"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime(a, "InputFormat", "MMMM d, yyyy", "TimeZone","Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime(a, "InputFormat", "yyyy-MM-dd", "TimeZone","Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime(a, "InputFormat", "yyyyMMdd", "TimeZone","Asia/Taipei")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.Month</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.Hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.Minute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x.Second</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>durations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start = "2022-02-01 14:00:23"
+end = "2022-03-03 15:12:23"
+製作 duration 格式物件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start = datetime(start, "InputFormat", "yyyyMMdd HH:mm:ss", "TimeZone","Asia/Taipei")
+end = datetime(end, "InputFormat", "yyyyMMdd HH:mm:ss", "TimeZone","Asia/Taipei")
+dur_length = end - start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉成間隔幾天？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>days(dur_length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉成間隔幾月？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉成間隔幾年？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉成間隔幾小時？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉成間隔幾分鐘？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轉成間隔幾秒？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>% 不可用 months(dur_length)，因為每個月長度不一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hours(dur_length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minutes(dur_length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seconds(dur_length)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以某天為基底，加減 duration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calendar duration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start = datetime(2022, 6, 3, 22, 00, 00)
+start + minutes(50) % 會變成 2022-06-03 22:50:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cal_dur = between(start, end)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1811,6 +2360,13 @@
       <family val="1"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體 (本文)"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1852,7 +2408,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1903,6 +2459,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2315,6 +2883,117 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF06F81D-7324-074E-A8BF-5AAE444A068E}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="64.1640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16">
+      <c r="A1" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16">
+      <c r="A6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16">
+      <c r="A7" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16">
+      <c r="A8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="80">
+      <c r="A9" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16">
+      <c r="A12" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16">
+      <c r="A14" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C168D83-819D-EA42-8E94-73A65D07DC4E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2362,7 +3041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE96BA2-E75F-5B49-AF81-9D22F0FC6C6F}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -2391,293 +3070,285 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8673484-8B2A-B34F-BC16-7F912DE56487}">
-  <dimension ref="A1:E47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50613941-3EEC-8548-9378-2F401ED715B3}">
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="59.6640625" customWidth="1"/>
-    <col min="4" max="5" width="58.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" style="17" customWidth="1"/>
+    <col min="2" max="4" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>21</v>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="17">
+        <v>20170131</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>23</v>
+        <v>345</v>
+      </c>
+      <c r="D3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="17" t="s">
+        <v>322</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>25</v>
+        <v>346</v>
+      </c>
+      <c r="D4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="17" t="s">
+        <v>354</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>347</v>
+      </c>
+      <c r="D5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="17" t="s">
+        <v>323</v>
+      </c>
       <c r="B6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>348</v>
+      </c>
+      <c r="D6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="17" t="s">
+        <v>324</v>
+      </c>
       <c r="B7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="32">
-      <c r="A11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>189</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="D7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="D8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>191</v>
-      </c>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="32">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="32">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" t="s">
+        <v>336</v>
+      </c>
+      <c r="D14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="B15" t="s">
+        <v>337</v>
+      </c>
+      <c r="D15" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="B16" t="s">
+        <v>338</v>
+      </c>
+      <c r="D16" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" t="s">
+        <v>339</v>
+      </c>
+      <c r="D17" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D18" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="B19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D19" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="19" t="s">
+        <v>334</v>
+      </c>
       <c r="B20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="128">
-      <c r="A24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="48">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="D27" s="5"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" ht="80">
-      <c r="A31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" ht="32">
-      <c r="A32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="5"/>
+        <v>342</v>
+      </c>
+      <c r="D20" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B21" t="s">
+        <v>343</v>
+      </c>
+      <c r="D21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B22" t="s">
+        <v>344</v>
+      </c>
+      <c r="D22" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="B26" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="80">
+      <c r="A27" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="D28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="D29" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D30" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="D31" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="D32" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="32">
-      <c r="A36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="48">
-      <c r="A37" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="32">
-      <c r="A38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="D47" s="5"/>
+      <c r="A33" s="17" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="32">
+      <c r="A34" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="48">
+      <c r="A38" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="D38" t="s">
+        <v>382</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2686,6 +3357,311 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8673484-8B2A-B34F-BC16-7F912DE56487}">
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="59.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="5" width="58.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="32">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="32">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="32">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="128">
+      <c r="A24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="48">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="D27" s="5"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" ht="80">
+      <c r="A31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" ht="32">
+      <c r="A32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="32">
+      <c r="A36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="48">
+      <c r="A37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="32">
+      <c r="A38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="D47" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48A1020-9B01-694E-8E90-619889560965}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2714,7 +3690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378D0CB2-1518-0A4F-B27C-E4EEE8F7CDAE}">
   <dimension ref="A1:B35"/>
   <sheetViews>
@@ -2952,12 +3928,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECF3FBE-13DA-7B41-AC08-FA89D30F5947}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A48" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2967,29 +3943,35 @@
     <col min="3" max="3" width="71.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="32">
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="32">
       <c r="B3" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="48">
+      <c r="D3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -2999,8 +3981,11 @@
       <c r="C4" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="48">
+      <c r="D4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="48">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -3011,7 +3996,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -3022,31 +4007,40 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="32">
+      <c r="D8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="32">
       <c r="B9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>234</v>
       </c>
@@ -3057,7 +4051,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>234</v>
       </c>
@@ -3068,7 +4062,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>234</v>
       </c>
@@ -3076,12 +4070,12 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="C13" s="7" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>234</v>
       </c>
@@ -3089,7 +4083,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="32">
+    <row r="15" spans="1:4" ht="32">
       <c r="A15" t="s">
         <v>236</v>
       </c>
@@ -3099,8 +4093,11 @@
       <c r="C15" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>236</v>
       </c>
@@ -3111,7 +4108,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="80">
+    <row r="17" spans="1:4" ht="80">
       <c r="A17" t="s">
         <v>237</v>
       </c>
@@ -3122,7 +4119,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="192">
+    <row r="18" spans="1:4" ht="192">
       <c r="B18" s="5" t="s">
         <v>46</v>
       </c>
@@ -3130,361 +4127,266 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="2" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>315</v>
+      </c>
+      <c r="D20" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="160">
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:4" ht="160">
+      <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C24" s="12" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="176">
-      <c r="B24" s="1"/>
-      <c r="C24" s="13" t="s">
+    <row r="25" spans="1:4" ht="176">
+      <c r="B25" s="1"/>
+      <c r="C25" s="13" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="96">
-      <c r="B25" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="48">
+    <row r="26" spans="1:4" ht="96">
       <c r="B26" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" ht="32">
+      <c r="C26" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="48">
       <c r="B27" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" ht="32">
+      <c r="B28" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="32">
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="1:4" ht="32">
+      <c r="B29" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32">
-      <c r="B29" s="1" t="s">
+    <row r="30" spans="1:4" ht="32">
+      <c r="B30" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="32">
-      <c r="B30" s="1" t="s">
+    <row r="31" spans="1:4" ht="32">
+      <c r="B31" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" ht="48">
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" ht="48">
+      <c r="B32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="32">
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="2:4" ht="32">
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="32">
-      <c r="B33" s="1" t="s">
+    <row r="34" spans="2:4" ht="32">
+      <c r="B34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="48">
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="2:4" ht="48">
+      <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="80">
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="2:4" ht="80">
+      <c r="B36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="16">
-      <c r="B36" s="1" t="s">
+    <row r="37" spans="2:4" ht="16">
+      <c r="B37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="16">
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="2:4" ht="16">
+      <c r="B38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="80">
-      <c r="B38" s="1" t="s">
+    <row r="39" spans="2:4" ht="80">
+      <c r="B39" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="2" t="s">
+    <row r="43" spans="2:4">
+      <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" ht="96">
-      <c r="B44" s="1" t="s">
+      <c r="D44" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="96">
+      <c r="B45" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C45" s="12" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" ht="96">
-      <c r="B45" s="1" t="s">
+      <c r="D45" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="96">
+      <c r="B46" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" ht="128">
-      <c r="B46" s="1" t="s">
+      <c r="D46" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="128">
+      <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" ht="96">
-      <c r="B47" s="1" t="s">
+      <c r="D47" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="96">
+      <c r="B48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="16">
-      <c r="B49" s="8" t="s">
+    <row r="50" spans="2:4" ht="16">
+      <c r="B50" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="48">
-      <c r="B51" s="11" t="s">
+    <row r="52" spans="2:4" ht="48">
+      <c r="B52" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C52" s="11" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" ht="48">
-      <c r="B52" s="1" t="s">
+      <c r="D52" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="48">
+      <c r="B53" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" ht="112">
-      <c r="B53" s="1" t="s">
+      <c r="D53" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="112">
+      <c r="B54" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="64">
-      <c r="B54" s="1" t="s">
+    <row r="55" spans="2:4" ht="64">
+      <c r="B55" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>225</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBA52E5-64CC-8A48-8D64-49D1DC6D7279}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="B11:C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" customWidth="1"/>
-    <col min="2" max="3" width="74.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="32">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="32">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="32">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="32">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="48">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="80">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="48">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="80">
-      <c r="B14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="64">
-      <c r="B15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3494,6 +4396,160 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBA52E5-64CC-8A48-8D64-49D1DC6D7279}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="2" max="3" width="74.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="32">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="32">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="32">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="48">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="80">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="48">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="80">
+      <c r="B14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="64">
+      <c r="B15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22F8C1-0FE9-8F4D-A6BD-B4FEFD648FF0}">
   <dimension ref="A1:D33"/>
   <sheetViews>
@@ -3685,7 +4741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCECF803-06B2-9641-AB22-9586B871C03C}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -3831,115 +4887,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF06F81D-7324-074E-A8BF-5AAE444A068E}">
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="64.1640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16">
-      <c r="A1" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16">
-      <c r="A3" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16">
-      <c r="A4" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16">
-      <c r="A5" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16">
-      <c r="A6" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16">
-      <c r="A7" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16">
-      <c r="A8" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="80">
-      <c r="A9" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16">
-      <c r="A12" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="16">
-      <c r="A14" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>